<commit_message>
Finalize for Session 2
Change Activities, add try catch to see where cabin picks aren't working, add some comments to explain why I did things or how to test things, change the output to do seperate sheets, update cabins for S2, etc...
</commit_message>
<xml_diff>
--- a/Activities.xlsx
+++ b/Activities.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Cabin</t>
   </si>
@@ -158,15 +158,9 @@
     <t>Lacrosse</t>
   </si>
   <si>
-    <t>Guitar</t>
-  </si>
-  <si>
     <t>OLS</t>
   </si>
   <si>
-    <t>Pottery</t>
-  </si>
-  <si>
     <t>Riflery</t>
   </si>
   <si>
@@ -185,9 +179,6 @@
     <t>Disc Golf</t>
   </si>
   <si>
-    <t>Horseback</t>
-  </si>
-  <si>
     <t>Flag Football</t>
   </si>
   <si>
@@ -195,6 +186,21 @@
   </si>
   <si>
     <t>Putt Putt</t>
+  </si>
+  <si>
+    <t>Thirtyone</t>
+  </si>
+  <si>
+    <t>Thirtytwo</t>
+  </si>
+  <si>
+    <t>Thirtythree</t>
+  </si>
+  <si>
+    <t>Thirtyfour</t>
+  </si>
+  <si>
+    <t>Thirtyfive</t>
   </si>
 </sst>
 </file>
@@ -509,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:W36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,7 +527,7 @@
     <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +565,7 @@
         <v>40</v>
       </c>
       <c r="M1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N1" t="s">
         <v>41</v>
@@ -589,19 +595,10 @@
         <v>49</v>
       </c>
       <c r="W1" t="s">
-        <v>50</v>
-      </c>
-      <c r="X1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y1" t="s">
         <v>52</v>
       </c>
-      <c r="Z1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -648,16 +645,13 @@
         <v>1</v>
       </c>
       <c r="P2">
-        <v>10</v>
-      </c>
-      <c r="Q2">
-        <v>8</v>
-      </c>
-      <c r="Z2">
+        <v>8</v>
+      </c>
+      <c r="W2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -676,20 +670,14 @@
       <c r="N3">
         <v>7</v>
       </c>
-      <c r="P3">
-        <v>5</v>
-      </c>
       <c r="R3">
-        <v>6</v>
-      </c>
-      <c r="T3">
         <v>65</v>
       </c>
-      <c r="U3">
+      <c r="S3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -711,23 +699,23 @@
       <c r="K4">
         <v>1</v>
       </c>
+      <c r="P4">
+        <v>6</v>
+      </c>
       <c r="Q4">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
       </c>
       <c r="S4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T4">
-        <v>2</v>
-      </c>
-      <c r="U4">
-        <v>4</v>
-      </c>
-      <c r="V4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -759,25 +747,19 @@
         <v>9</v>
       </c>
       <c r="P5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="Q5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S5">
-        <v>7</v>
-      </c>
-      <c r="T5">
-        <v>5</v>
-      </c>
-      <c r="U5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -802,20 +784,20 @@
       <c r="O6">
         <v>1</v>
       </c>
+      <c r="P6">
+        <v>7</v>
+      </c>
       <c r="Q6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="S6">
-        <v>3</v>
-      </c>
-      <c r="U6">
-        <v>8</v>
-      </c>
-      <c r="V6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="T6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -844,13 +826,10 @@
         <v>7</v>
       </c>
       <c r="P7">
-        <v>4</v>
-      </c>
-      <c r="Q7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -881,20 +860,20 @@
       <c r="O8">
         <v>2</v>
       </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
       <c r="Q8">
-        <v>5</v>
-      </c>
-      <c r="S8">
-        <v>7</v>
-      </c>
-      <c r="T8">
-        <v>6</v>
-      </c>
-      <c r="Z8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="W8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -935,15 +914,12 @@
         <v>3</v>
       </c>
       <c r="P9">
-        <v>2</v>
-      </c>
-      <c r="Q9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -964,19 +940,16 @@
         <v>1</v>
       </c>
       <c r="R10">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
       </c>
       <c r="T10">
-        <v>7</v>
-      </c>
-      <c r="U10">
-        <v>2</v>
-      </c>
-      <c r="V10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1011,16 +984,10 @@
         <v>3</v>
       </c>
       <c r="P11">
-        <v>6</v>
-      </c>
-      <c r="Q11">
         <v>4</v>
       </c>
-      <c r="R11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1049,22 +1016,16 @@
         <v>4</v>
       </c>
       <c r="P12">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R12">
-        <v>8</v>
-      </c>
-      <c r="S12">
-        <v>6</v>
-      </c>
-      <c r="T12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1090,16 +1051,10 @@
         <v>7</v>
       </c>
       <c r="P13">
-        <v>8</v>
-      </c>
-      <c r="Q13">
-        <v>10</v>
-      </c>
-      <c r="R13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1124,17 +1079,23 @@
       <c r="O14">
         <v>7</v>
       </c>
+      <c r="P14">
+        <v>8</v>
+      </c>
       <c r="Q14">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S14">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="T14">
+        <v>11</v>
       </c>
       <c r="U14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1154,22 +1115,16 @@
         <v>5</v>
       </c>
       <c r="P15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q15">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="R15">
-        <v>8</v>
-      </c>
-      <c r="S15">
-        <v>9</v>
-      </c>
-      <c r="T15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1194,17 +1149,11 @@
       <c r="N16">
         <v>8</v>
       </c>
-      <c r="P16">
-        <v>7</v>
-      </c>
       <c r="R16">
-        <v>9</v>
-      </c>
-      <c r="T16">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1244,78 +1193,1607 @@
       <c r="M17">
         <v>10</v>
       </c>
-      <c r="Q17">
+      <c r="P17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="W17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <f>B18+1</f>
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:P18" si="0">C18+1</f>
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="Q18">
+        <f>P18+1</f>
+        <v>16</v>
+      </c>
+      <c r="R18">
+        <f>Q18+1</f>
+        <v>17</v>
+      </c>
+      <c r="S18">
+        <f>R18+1</f>
+        <v>18</v>
+      </c>
+      <c r="T18">
+        <f>S18+1</f>
+        <v>19</v>
+      </c>
+      <c r="W18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f t="shared" ref="B19:B36" ca="1" si="1">RANDBETWEEN(1,6)</f>
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:Q19" ca="1" si="2">B19+1</f>
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="J19">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="L19">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="M19">
+        <f t="shared" ca="1" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ca="1" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="P19">
+        <f t="shared" ca="1" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" ca="1" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="R19">
+        <f ca="1">Q19+1</f>
+        <v>18</v>
+      </c>
+      <c r="S19">
+        <f ca="1">R19+1</f>
+        <v>19</v>
+      </c>
+      <c r="T19">
+        <f ca="1">S19+1</f>
+        <v>20</v>
+      </c>
+      <c r="W19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:Q20" ca="1" si="3">B20+1</f>
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ca="1" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ca="1" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="J20">
+        <f t="shared" ca="1" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="K20">
+        <f t="shared" ca="1" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ca="1" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="M20">
+        <f t="shared" ca="1" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ca="1" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="O20">
+        <f t="shared" ca="1" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="P20">
+        <f t="shared" ca="1" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" ca="1" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="R20">
+        <f ca="1">Q20+1</f>
+        <v>21</v>
+      </c>
+      <c r="S20">
+        <f ca="1">R20+1</f>
+        <v>22</v>
+      </c>
+      <c r="T20">
+        <f ca="1">S20+1</f>
+        <v>23</v>
+      </c>
+      <c r="W20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:Q21" ca="1" si="4">B21+1</f>
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ca="1" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ca="1" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="J21">
+        <f t="shared" ca="1" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ca="1" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ca="1" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="M21">
+        <f t="shared" ca="1" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ca="1" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="O21">
+        <f t="shared" ca="1" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="P21">
+        <f t="shared" ca="1" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" ca="1" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="R21">
+        <f ca="1">Q21+1</f>
+        <v>19</v>
+      </c>
+      <c r="S21">
+        <f ca="1">R21+1</f>
+        <v>20</v>
+      </c>
+      <c r="T21">
+        <f ca="1">S21+1</f>
+        <v>21</v>
+      </c>
+      <c r="W21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:Q22" ca="1" si="5">B22+1</f>
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ca="1" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ca="1" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ca="1" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ca="1" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ca="1" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ca="1" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="L22">
+        <f t="shared" ca="1" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="M22">
+        <f t="shared" ca="1" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ca="1" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="O22">
+        <f t="shared" ca="1" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="P22">
+        <f t="shared" ca="1" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" ca="1" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="R22">
+        <f ca="1">Q22+1</f>
+        <v>22</v>
+      </c>
+      <c r="S22">
+        <f ca="1">R22+1</f>
+        <v>23</v>
+      </c>
+      <c r="T22">
+        <f ca="1">S22+1</f>
+        <v>24</v>
+      </c>
+      <c r="W22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:Q23" ca="1" si="6">B23+1</f>
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ca="1" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ca="1" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ca="1" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ca="1" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ca="1" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ca="1" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ca="1" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ca="1" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ca="1" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ca="1" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="P23">
+        <f t="shared" ca="1" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" ca="1" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="R23">
+        <f ca="1">Q23+1</f>
+        <v>17</v>
+      </c>
+      <c r="S23">
+        <f ca="1">R23+1</f>
+        <v>18</v>
+      </c>
+      <c r="T23">
+        <f ca="1">S23+1</f>
+        <v>19</v>
+      </c>
+      <c r="W23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:Q24" ca="1" si="7">B24+1</f>
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ca="1" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ca="1" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ca="1" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ca="1" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ca="1" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <f t="shared" ca="1" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ca="1" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="K24">
+        <f t="shared" ca="1" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ca="1" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ca="1" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="N24">
+        <f t="shared" ca="1" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="O24">
+        <f t="shared" ca="1" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="P24">
+        <f t="shared" ca="1" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" ca="1" si="7"/>
+        <v>19</v>
+      </c>
+      <c r="R24">
+        <f ca="1">Q24+1</f>
+        <v>20</v>
+      </c>
+      <c r="S24">
+        <f ca="1">R24+1</f>
+        <v>21</v>
+      </c>
+      <c r="T24">
+        <f ca="1">S24+1</f>
+        <v>22</v>
+      </c>
+      <c r="W24">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:Q25" ca="1" si="8">B25+1</f>
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ca="1" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ca="1" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ca="1" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ca="1" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ca="1" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <f t="shared" ca="1" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="J25">
+        <f t="shared" ca="1" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="K25">
+        <f t="shared" ca="1" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ca="1" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ca="1" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ca="1" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="O25">
+        <f t="shared" ca="1" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="P25">
+        <f t="shared" ca="1" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" ca="1" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="R25">
+        <f ca="1">Q25+1</f>
+        <v>18</v>
+      </c>
+      <c r="S25">
+        <f ca="1">R25+1</f>
+        <v>19</v>
+      </c>
+      <c r="T25">
+        <f ca="1">S25+1</f>
+        <v>20</v>
+      </c>
+      <c r="W25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:Q26" ca="1" si="9">B26+1</f>
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ca="1" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ca="1" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ca="1" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ca="1" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="H26">
+        <f t="shared" ca="1" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="I26">
+        <f t="shared" ca="1" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="J26">
+        <f t="shared" ca="1" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="K26">
+        <f t="shared" ca="1" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="L26">
+        <f t="shared" ca="1" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="M26">
+        <f t="shared" ca="1" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ca="1" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="O26">
+        <f t="shared" ca="1" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="P26">
+        <f t="shared" ca="1" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" ca="1" si="9"/>
+        <v>17</v>
+      </c>
+      <c r="R26">
+        <f ca="1">Q26+1</f>
+        <v>18</v>
+      </c>
+      <c r="S26">
+        <f ca="1">R26+1</f>
+        <v>19</v>
+      </c>
+      <c r="T26">
+        <f ca="1">S26+1</f>
+        <v>20</v>
+      </c>
+      <c r="W26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27:Q27" ca="1" si="10">B27+1</f>
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ca="1" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ca="1" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ca="1" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <f t="shared" ca="1" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ca="1" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ca="1" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ca="1" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ca="1" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="L27">
+        <f t="shared" ca="1" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ca="1" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ca="1" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ca="1" si="10"/>
+        <v>17</v>
+      </c>
+      <c r="P27">
+        <f t="shared" ca="1" si="10"/>
+        <v>18</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" ca="1" si="10"/>
+        <v>19</v>
+      </c>
+      <c r="R27">
+        <f ca="1">Q27+1</f>
+        <v>20</v>
+      </c>
+      <c r="S27">
+        <f ca="1">R27+1</f>
+        <v>21</v>
+      </c>
+      <c r="T27">
+        <f ca="1">S27+1</f>
+        <v>22</v>
+      </c>
+      <c r="W27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:Q28" ca="1" si="11">B28+1</f>
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ca="1" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <f t="shared" ca="1" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ca="1" si="11"/>
+        <v>10</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ca="1" si="11"/>
+        <v>11</v>
+      </c>
+      <c r="H28">
+        <f t="shared" ca="1" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="I28">
+        <f t="shared" ca="1" si="11"/>
+        <v>13</v>
+      </c>
+      <c r="J28">
+        <f t="shared" ca="1" si="11"/>
+        <v>14</v>
+      </c>
+      <c r="K28">
+        <f t="shared" ca="1" si="11"/>
+        <v>15</v>
+      </c>
+      <c r="L28">
+        <f t="shared" ca="1" si="11"/>
+        <v>16</v>
+      </c>
+      <c r="M28">
+        <f t="shared" ca="1" si="11"/>
+        <v>17</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ca="1" si="11"/>
+        <v>18</v>
+      </c>
+      <c r="O28">
+        <f t="shared" ca="1" si="11"/>
+        <v>19</v>
+      </c>
+      <c r="P28">
+        <f t="shared" ca="1" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" ca="1" si="11"/>
+        <v>21</v>
+      </c>
+      <c r="R28">
+        <f ca="1">Q28+1</f>
+        <v>22</v>
+      </c>
+      <c r="S28">
+        <f ca="1">R28+1</f>
+        <v>23</v>
+      </c>
+      <c r="T28">
+        <f ca="1">S28+1</f>
+        <v>24</v>
+      </c>
+      <c r="W28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:Q29" ca="1" si="12">B29+1</f>
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ca="1" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ca="1" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ca="1" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ca="1" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ca="1" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="I29">
+        <f t="shared" ca="1" si="12"/>
+        <v>11</v>
+      </c>
+      <c r="J29">
+        <f t="shared" ca="1" si="12"/>
+        <v>12</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ca="1" si="12"/>
+        <v>13</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ca="1" si="12"/>
+        <v>14</v>
+      </c>
+      <c r="M29">
+        <f t="shared" ca="1" si="12"/>
+        <v>15</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ca="1" si="12"/>
+        <v>16</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ca="1" si="12"/>
+        <v>17</v>
+      </c>
+      <c r="P29">
+        <f t="shared" ca="1" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" ca="1" si="12"/>
+        <v>19</v>
+      </c>
+      <c r="R29">
+        <f ca="1">Q29+1</f>
+        <v>20</v>
+      </c>
+      <c r="S29">
+        <f ca="1">R29+1</f>
+        <v>21</v>
+      </c>
+      <c r="T29">
+        <f ca="1">S29+1</f>
+        <v>22</v>
+      </c>
+      <c r="W29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:Q30" ca="1" si="13">B30+1</f>
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ca="1" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ca="1" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ca="1" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ca="1" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <f t="shared" ca="1" si="13"/>
+        <v>11</v>
+      </c>
+      <c r="I30">
+        <f t="shared" ca="1" si="13"/>
+        <v>12</v>
+      </c>
+      <c r="J30">
+        <f t="shared" ca="1" si="13"/>
+        <v>13</v>
+      </c>
+      <c r="K30">
+        <f t="shared" ca="1" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="L30">
+        <f t="shared" ca="1" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="M30">
+        <f t="shared" ca="1" si="13"/>
+        <v>16</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ca="1" si="13"/>
+        <v>17</v>
+      </c>
+      <c r="O30">
+        <f t="shared" ca="1" si="13"/>
+        <v>18</v>
+      </c>
+      <c r="P30">
+        <f t="shared" ca="1" si="13"/>
+        <v>19</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" ca="1" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="R30">
+        <f ca="1">Q30+1</f>
+        <v>21</v>
+      </c>
+      <c r="S30">
+        <f ca="1">R30+1</f>
+        <v>22</v>
+      </c>
+      <c r="T30">
+        <f ca="1">S30+1</f>
+        <v>23</v>
+      </c>
+      <c r="W30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
+      </c>
+      <c r="B31">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:Q31" ca="1" si="14">B31+1</f>
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ca="1" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <f t="shared" ca="1" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="F31">
+        <f t="shared" ca="1" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="G31">
+        <f t="shared" ca="1" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ca="1" si="14"/>
+        <v>11</v>
+      </c>
+      <c r="I31">
+        <f t="shared" ca="1" si="14"/>
+        <v>12</v>
+      </c>
+      <c r="J31">
+        <f t="shared" ca="1" si="14"/>
+        <v>13</v>
+      </c>
+      <c r="K31">
+        <f t="shared" ca="1" si="14"/>
+        <v>14</v>
+      </c>
+      <c r="L31">
+        <f t="shared" ca="1" si="14"/>
+        <v>15</v>
+      </c>
+      <c r="M31">
+        <f t="shared" ca="1" si="14"/>
+        <v>16</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ca="1" si="14"/>
+        <v>17</v>
+      </c>
+      <c r="O31">
+        <f t="shared" ca="1" si="14"/>
+        <v>18</v>
+      </c>
+      <c r="P31">
+        <f t="shared" ca="1" si="14"/>
+        <v>19</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" ca="1" si="14"/>
+        <v>20</v>
+      </c>
+      <c r="R31">
+        <f ca="1">Q31+1</f>
+        <v>21</v>
+      </c>
+      <c r="S31">
+        <f ca="1">R31+1</f>
+        <v>22</v>
+      </c>
+      <c r="T31">
+        <f ca="1">S31+1</f>
+        <v>23</v>
+      </c>
+      <c r="W31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:Q32" ca="1" si="15">B32+1</f>
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ca="1" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <f t="shared" ca="1" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="F32">
+        <f t="shared" ca="1" si="15"/>
+        <v>7</v>
+      </c>
+      <c r="G32">
+        <f t="shared" ca="1" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <f t="shared" ca="1" si="15"/>
+        <v>9</v>
+      </c>
+      <c r="I32">
+        <f t="shared" ca="1" si="15"/>
+        <v>10</v>
+      </c>
+      <c r="J32">
+        <f t="shared" ca="1" si="15"/>
+        <v>11</v>
+      </c>
+      <c r="K32">
+        <f t="shared" ca="1" si="15"/>
+        <v>12</v>
+      </c>
+      <c r="L32">
+        <f t="shared" ca="1" si="15"/>
+        <v>13</v>
+      </c>
+      <c r="M32">
+        <f t="shared" ca="1" si="15"/>
+        <v>14</v>
+      </c>
+      <c r="N32">
+        <f t="shared" ca="1" si="15"/>
+        <v>15</v>
+      </c>
+      <c r="O32">
+        <f t="shared" ca="1" si="15"/>
+        <v>16</v>
+      </c>
+      <c r="P32">
+        <f t="shared" ca="1" si="15"/>
+        <v>17</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" ca="1" si="15"/>
+        <v>18</v>
+      </c>
+      <c r="R32">
+        <f ca="1">Q32+1</f>
+        <v>19</v>
+      </c>
+      <c r="S32">
+        <f ca="1">R32+1</f>
+        <v>20</v>
+      </c>
+      <c r="T32">
+        <f ca="1">S32+1</f>
+        <v>21</v>
+      </c>
+      <c r="W32">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:Q33" ca="1" si="16">B33+1</f>
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ca="1" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <f t="shared" ca="1" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ca="1" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ca="1" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="H33">
+        <f t="shared" ca="1" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="I33">
+        <f t="shared" ca="1" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="J33">
+        <f t="shared" ca="1" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="K33">
+        <f t="shared" ca="1" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="L33">
+        <f t="shared" ca="1" si="16"/>
+        <v>11</v>
+      </c>
+      <c r="M33">
+        <f t="shared" ca="1" si="16"/>
+        <v>12</v>
+      </c>
+      <c r="N33">
+        <f t="shared" ca="1" si="16"/>
+        <v>13</v>
+      </c>
+      <c r="O33">
+        <f t="shared" ca="1" si="16"/>
+        <v>14</v>
+      </c>
+      <c r="P33">
+        <f t="shared" ca="1" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" ca="1" si="16"/>
+        <v>16</v>
+      </c>
+      <c r="R33">
+        <f ca="1">Q33+1</f>
+        <v>17</v>
+      </c>
+      <c r="S33">
+        <f ca="1">R33+1</f>
+        <v>18</v>
+      </c>
+      <c r="T33">
+        <f ca="1">S33+1</f>
+        <v>19</v>
+      </c>
+      <c r="W33">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:Q34" ca="1" si="17">B34+1</f>
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ca="1" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ca="1" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ca="1" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ca="1" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ca="1" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="I34">
+        <f t="shared" ca="1" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="J34">
+        <f t="shared" ca="1" si="17"/>
+        <v>11</v>
+      </c>
+      <c r="K34">
+        <f t="shared" ca="1" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="L34">
+        <f t="shared" ca="1" si="17"/>
+        <v>13</v>
+      </c>
+      <c r="M34">
+        <f t="shared" ca="1" si="17"/>
+        <v>14</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ca="1" si="17"/>
+        <v>15</v>
+      </c>
+      <c r="O34">
+        <f t="shared" ca="1" si="17"/>
+        <v>16</v>
+      </c>
+      <c r="P34">
+        <f t="shared" ca="1" si="17"/>
+        <v>17</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" ca="1" si="17"/>
+        <v>18</v>
+      </c>
+      <c r="R34">
+        <f ca="1">Q34+1</f>
+        <v>19</v>
+      </c>
+      <c r="S34">
+        <f ca="1">R34+1</f>
+        <v>20</v>
+      </c>
+      <c r="T34">
+        <f ca="1">S34+1</f>
+        <v>21</v>
+      </c>
+      <c r="W34">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:Q35" ca="1" si="18">B35+1</f>
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ca="1" si="18"/>
+        <v>7</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ca="1" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ca="1" si="18"/>
+        <v>9</v>
+      </c>
+      <c r="G35">
+        <f t="shared" ca="1" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ca="1" si="18"/>
+        <v>11</v>
+      </c>
+      <c r="I35">
+        <f t="shared" ca="1" si="18"/>
+        <v>12</v>
+      </c>
+      <c r="J35">
+        <f t="shared" ca="1" si="18"/>
+        <v>13</v>
+      </c>
+      <c r="K35">
+        <f t="shared" ca="1" si="18"/>
+        <v>14</v>
+      </c>
+      <c r="L35">
+        <f t="shared" ca="1" si="18"/>
+        <v>15</v>
+      </c>
+      <c r="M35">
+        <f t="shared" ca="1" si="18"/>
+        <v>16</v>
+      </c>
+      <c r="N35">
+        <f t="shared" ca="1" si="18"/>
+        <v>17</v>
+      </c>
+      <c r="O35">
+        <f t="shared" ca="1" si="18"/>
+        <v>18</v>
+      </c>
+      <c r="P35">
+        <f t="shared" ca="1" si="18"/>
+        <v>19</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" ca="1" si="18"/>
+        <v>20</v>
+      </c>
+      <c r="R35">
+        <f ca="1">Q35+1</f>
+        <v>21</v>
+      </c>
+      <c r="S35">
+        <f ca="1">R35+1</f>
+        <v>22</v>
+      </c>
+      <c r="T35">
+        <f ca="1">S35+1</f>
+        <v>23</v>
+      </c>
+      <c r="W35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:Q36" ca="1" si="19">B36+1</f>
+        <v>6</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ca="1" si="19"/>
+        <v>7</v>
+      </c>
+      <c r="E36">
+        <f t="shared" ca="1" si="19"/>
+        <v>8</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ca="1" si="19"/>
+        <v>9</v>
+      </c>
+      <c r="G36">
+        <f t="shared" ca="1" si="19"/>
+        <v>10</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ca="1" si="19"/>
+        <v>11</v>
+      </c>
+      <c r="I36">
+        <f t="shared" ca="1" si="19"/>
+        <v>12</v>
+      </c>
+      <c r="J36">
+        <f t="shared" ca="1" si="19"/>
+        <v>13</v>
+      </c>
+      <c r="K36">
+        <f t="shared" ca="1" si="19"/>
+        <v>14</v>
+      </c>
+      <c r="L36">
+        <f t="shared" ca="1" si="19"/>
+        <v>15</v>
+      </c>
+      <c r="M36">
+        <f t="shared" ca="1" si="19"/>
+        <v>16</v>
+      </c>
+      <c r="N36">
+        <f t="shared" ca="1" si="19"/>
+        <v>17</v>
+      </c>
+      <c r="O36">
+        <f t="shared" ca="1" si="19"/>
+        <v>18</v>
+      </c>
+      <c r="P36">
+        <f t="shared" ca="1" si="19"/>
+        <v>19</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" ca="1" si="19"/>
+        <v>20</v>
+      </c>
+      <c r="R36">
+        <f ca="1">Q36+1</f>
+        <v>21</v>
+      </c>
+      <c r="S36">
+        <f ca="1">R36+1</f>
+        <v>22</v>
+      </c>
+      <c r="T36">
+        <f ca="1">S36+1</f>
+        <v>23</v>
+      </c>
+      <c r="W36">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>